<commit_message>
On/Off by Sensors done
</commit_message>
<xml_diff>
--- a/Calculations.xlsx
+++ b/Calculations.xlsx
@@ -441,7 +441,7 @@
   <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -584,7 +584,7 @@
         <v>18</v>
       </c>
       <c r="B19">
-        <v>9.1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -609,7 +609,7 @@
       </c>
       <c r="B22">
         <f>(B19/B20)*B21+B21</f>
-        <v>4.4400000000000004</v>
+        <v>4.8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>